<commit_message>
Merged PR 7738: Fixed issue, where when searching for a station by call letters, the wrong field was used
Fixed issue, where when searching for a station by call letters, the station_call_letters was used instead of legacy_call_letters.
Fixed, and updated tests.
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ProprietaryDataFiles/Barter_ValidFormat_SpotLengthWithColon.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ProprietaryDataFiles/Barter_ValidFormat_SpotLengthWithColon.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bbotelho\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\BarterDataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferenc.pato\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A3F43E5-5F8C-4C7A-A565-84B8195A841E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E09745-A1BF-4FB5-8622-3AB509159C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barter Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Barter Header</t>
   </si>
@@ -185,15 +193,6 @@
   </si>
   <si>
     <t>Comment 4</t>
-  </si>
-  <si>
-    <t>EESH-TV 69.2</t>
-  </si>
-  <si>
-    <t>W-F 3-4A</t>
-  </si>
-  <si>
-    <t>Comment 5</t>
   </si>
   <si>
     <t>TTWN</t>
@@ -770,26 +769,26 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1339,7 +1338,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="17" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -1385,19 +1384,19 @@
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="38" t="str">
         <f>IF(COUNTA($E$3:$E12) &gt; 0, "Errors", "")</f>
         <v>Errors</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1420,20 +1419,20 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="31" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="33"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1458,18 +1457,18 @@
       <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="31" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="33"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1494,18 +1493,18 @@
       <c r="B5" s="9">
         <v>43496</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="31" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="33"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1530,18 +1529,18 @@
       <c r="B6" s="9">
         <v>43829</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="31" t="s">
+      <c r="D6" s="32"/>
+      <c r="E6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="33"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="37"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1566,18 +1565,18 @@
       <c r="B7" s="10">
         <v>99.88</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="31" t="s">
+      <c r="D7" s="32"/>
+      <c r="E7" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="33"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="37"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1602,16 +1601,16 @@
       <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="33"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="37"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1636,16 +1635,16 @@
       <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="33"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="37"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1670,16 +1669,16 @@
       <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="33"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="37"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1704,16 +1703,16 @@
       <c r="B11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="33"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="37"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1738,18 +1737,18 @@
       <c r="B12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="31" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="33"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="37"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -2143,36 +2142,16 @@
       <c r="Z21" s="17"/>
     </row>
     <row r="22" spans="1:26" ht="24" customHeight="1">
-      <c r="A22" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="17">
-        <v>1</v>
-      </c>
-      <c r="D22" s="17">
-        <v>4</v>
-      </c>
-      <c r="E22" s="17">
-        <v>3</v>
-      </c>
-      <c r="F22" s="17">
-        <v>5</v>
-      </c>
-      <c r="G22" s="17">
-        <v>1</v>
-      </c>
-      <c r="H22" s="17">
-        <v>4</v>
-      </c>
-      <c r="I22" s="17">
-        <v>3</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
       <c r="K22" s="30"/>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
@@ -29576,28 +29555,28 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="E2:J2"/>
     <mergeCell ref="E8:J8"/>
     <mergeCell ref="E9:J9"/>
     <mergeCell ref="E7:J7"/>
     <mergeCell ref="E3:J3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <conditionalFormatting sqref="B11">
     <cfRule type="expression" dxfId="20" priority="1">

</xml_diff>